<commit_message>
SUM by excel formula
</commit_message>
<xml_diff>
--- a/xtt_demo/02-01_R.xlsx
+++ b/xtt_demo/02-01_R.xlsx
@@ -3394,7 +3394,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="9">
-        <v>44010.000000000000</v>
+        <v>44013.000000000000</v>
       </c>
       <c r="E5" s="8">
         <v>6758.57</v>
@@ -3411,7 +3411,7 @@
         <v>25</v>
       </c>
       <c r="D6" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E6" s="8">
         <v>982.68</v>
@@ -3428,7 +3428,7 @@
         <v>28</v>
       </c>
       <c r="D7" s="9">
-        <v>44010.000000000000</v>
+        <v>44013.000000000000</v>
       </c>
       <c r="E7" s="8">
         <v>6836.72</v>
@@ -3445,7 +3445,7 @@
         <v>28</v>
       </c>
       <c r="D8" s="9">
-        <v>44010.000000000000</v>
+        <v>44013.000000000000</v>
       </c>
       <c r="E8" s="8">
         <v>4038.64</v>
@@ -3462,7 +3462,7 @@
         <v>25</v>
       </c>
       <c r="D9" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E9" s="8">
         <v>7630.05</v>
@@ -3479,7 +3479,7 @@
         <v>28</v>
       </c>
       <c r="D10" s="9">
-        <v>44010.000000000000</v>
+        <v>44013.000000000000</v>
       </c>
       <c r="E10" s="8">
         <v>5746.69</v>
@@ -3496,7 +3496,7 @@
         <v>28</v>
       </c>
       <c r="D11" s="9">
-        <v>44010.000000000000</v>
+        <v>44013.000000000000</v>
       </c>
       <c r="E11" s="8">
         <v>471.62</v>
@@ -3513,7 +3513,7 @@
         <v>25</v>
       </c>
       <c r="D12" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E12" s="8">
         <v>6001.36</v>
@@ -3530,7 +3530,7 @@
         <v>27</v>
       </c>
       <c r="D13" s="9">
-        <v>44011.000000000000</v>
+        <v>44014.000000000000</v>
       </c>
       <c r="E13" s="8">
         <v>9950.90</v>
@@ -3547,7 +3547,7 @@
         <v>26</v>
       </c>
       <c r="D14" s="9">
-        <v>44012.000000000000</v>
+        <v>44015.000000000000</v>
       </c>
       <c r="E14" s="8">
         <v>153.90</v>
@@ -3564,7 +3564,7 @@
         <v>25</v>
       </c>
       <c r="D15" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E15" s="8">
         <v>8972.09</v>
@@ -3581,7 +3581,7 @@
         <v>27</v>
       </c>
       <c r="D16" s="9">
-        <v>44011.000000000000</v>
+        <v>44014.000000000000</v>
       </c>
       <c r="E16" s="8">
         <v>214.52</v>
@@ -3598,7 +3598,7 @@
         <v>26</v>
       </c>
       <c r="D17" s="9">
-        <v>44012.000000000000</v>
+        <v>44015.000000000000</v>
       </c>
       <c r="E17" s="8">
         <v>4164.85</v>
@@ -3615,7 +3615,7 @@
         <v>25</v>
       </c>
       <c r="D18" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E18" s="8">
         <v>847.44</v>
@@ -3632,7 +3632,7 @@
         <v>27</v>
       </c>
       <c r="D19" s="9">
-        <v>44011.000000000000</v>
+        <v>44014.000000000000</v>
       </c>
       <c r="E19" s="8">
         <v>6220.04</v>
@@ -3700,7 +3700,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="13">
-        <v>44010.000000000000</v>
+        <v>44013.000000000000</v>
       </c>
       <c r="E5" s="14">
         <v>6758.57</v>
@@ -3717,7 +3717,7 @@
         <v>25</v>
       </c>
       <c r="D6" s="13">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E6" s="14">
         <v>982.68</v>
@@ -3734,7 +3734,7 @@
         <v>28</v>
       </c>
       <c r="D7" s="13">
-        <v>44010.000000000000</v>
+        <v>44013.000000000000</v>
       </c>
       <c r="E7" s="14">
         <v>6836.72</v>
@@ -3751,7 +3751,7 @@
         <v>28</v>
       </c>
       <c r="D8" s="13">
-        <v>44010.000000000000</v>
+        <v>44013.000000000000</v>
       </c>
       <c r="E8" s="14">
         <v>4038.64</v>
@@ -3768,7 +3768,7 @@
         <v>25</v>
       </c>
       <c r="D9" s="13">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E9" s="14">
         <v>7630.05</v>
@@ -3785,7 +3785,7 @@
         <v>28</v>
       </c>
       <c r="D10" s="13">
-        <v>44010.000000000000</v>
+        <v>44013.000000000000</v>
       </c>
       <c r="E10" s="14">
         <v>5746.69</v>
@@ -3802,7 +3802,7 @@
         <v>28</v>
       </c>
       <c r="D11" s="13">
-        <v>44010.000000000000</v>
+        <v>44013.000000000000</v>
       </c>
       <c r="E11" s="14">
         <v>471.62</v>
@@ -3819,7 +3819,7 @@
         <v>25</v>
       </c>
       <c r="D12" s="13">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E12" s="14">
         <v>6001.36</v>
@@ -3836,7 +3836,7 @@
         <v>27</v>
       </c>
       <c r="D13" s="13">
-        <v>44011.000000000000</v>
+        <v>44014.000000000000</v>
       </c>
       <c r="E13" s="14">
         <v>9950.90</v>
@@ -3853,7 +3853,7 @@
         <v>26</v>
       </c>
       <c r="D14" s="13">
-        <v>44012.000000000000</v>
+        <v>44015.000000000000</v>
       </c>
       <c r="E14" s="14">
         <v>153.90</v>
@@ -3870,7 +3870,7 @@
         <v>25</v>
       </c>
       <c r="D15" s="13">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E15" s="14">
         <v>8972.09</v>
@@ -3887,7 +3887,7 @@
         <v>27</v>
       </c>
       <c r="D16" s="13">
-        <v>44011.000000000000</v>
+        <v>44014.000000000000</v>
       </c>
       <c r="E16" s="14">
         <v>214.52</v>
@@ -3904,7 +3904,7 @@
         <v>26</v>
       </c>
       <c r="D17" s="13">
-        <v>44012.000000000000</v>
+        <v>44015.000000000000</v>
       </c>
       <c r="E17" s="14">
         <v>4164.85</v>
@@ -3921,7 +3921,7 @@
         <v>25</v>
       </c>
       <c r="D18" s="13">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E18" s="14">
         <v>847.44</v>
@@ -3938,7 +3938,7 @@
         <v>27</v>
       </c>
       <c r="D19" s="13">
-        <v>44011.000000000000</v>
+        <v>44014.000000000000</v>
       </c>
       <c r="E19" s="14">
         <v>6220.04</v>
@@ -4114,7 +4114,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="9">
-        <v>44010.000000000000</v>
+        <v>44013.000000000000</v>
       </c>
       <c r="E5" s="8">
         <v>6758.57</v>
@@ -4132,7 +4132,7 @@
         <v>25</v>
       </c>
       <c r="D6" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E6" s="8">
         <v>982.68</v>
@@ -4150,7 +4150,7 @@
         <v>28</v>
       </c>
       <c r="D7" s="9">
-        <v>44010.000000000000</v>
+        <v>44013.000000000000</v>
       </c>
       <c r="E7" s="8">
         <v>6836.72</v>
@@ -4168,7 +4168,7 @@
         <v>28</v>
       </c>
       <c r="D8" s="9">
-        <v>44010.000000000000</v>
+        <v>44013.000000000000</v>
       </c>
       <c r="E8" s="8">
         <v>4038.64</v>
@@ -4186,7 +4186,7 @@
         <v>25</v>
       </c>
       <c r="D9" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E9" s="8">
         <v>7630.05</v>
@@ -4204,7 +4204,7 @@
         <v>28</v>
       </c>
       <c r="D10" s="9">
-        <v>44010.000000000000</v>
+        <v>44013.000000000000</v>
       </c>
       <c r="E10" s="8">
         <v>5746.69</v>
@@ -4222,7 +4222,7 @@
         <v>28</v>
       </c>
       <c r="D11" s="9">
-        <v>44010.000000000000</v>
+        <v>44013.000000000000</v>
       </c>
       <c r="E11" s="8">
         <v>471.62</v>
@@ -4240,7 +4240,7 @@
         <v>25</v>
       </c>
       <c r="D12" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E12" s="8">
         <v>6001.36</v>
@@ -4258,7 +4258,7 @@
         <v>27</v>
       </c>
       <c r="D13" s="9">
-        <v>44011.000000000000</v>
+        <v>44014.000000000000</v>
       </c>
       <c r="E13" s="8">
         <v>9950.90</v>
@@ -4276,7 +4276,7 @@
         <v>26</v>
       </c>
       <c r="D14" s="9">
-        <v>44012.000000000000</v>
+        <v>44015.000000000000</v>
       </c>
       <c r="E14" s="8">
         <v>153.90</v>
@@ -4294,7 +4294,7 @@
         <v>25</v>
       </c>
       <c r="D15" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E15" s="8">
         <v>8972.09</v>
@@ -4312,7 +4312,7 @@
         <v>27</v>
       </c>
       <c r="D16" s="9">
-        <v>44011.000000000000</v>
+        <v>44014.000000000000</v>
       </c>
       <c r="E16" s="8">
         <v>214.52</v>
@@ -4330,7 +4330,7 @@
         <v>26</v>
       </c>
       <c r="D17" s="9">
-        <v>44012.000000000000</v>
+        <v>44015.000000000000</v>
       </c>
       <c r="E17" s="8">
         <v>4164.85</v>
@@ -4348,7 +4348,7 @@
         <v>25</v>
       </c>
       <c r="D18" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E18" s="8">
         <v>847.44</v>
@@ -4366,7 +4366,7 @@
         <v>27</v>
       </c>
       <c r="D19" s="9">
-        <v>44011.000000000000</v>
+        <v>44014.000000000000</v>
       </c>
       <c r="E19" s="8">
         <v>6220.04</v>
@@ -4461,7 +4461,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="9">
-        <v>44010.000000000000</v>
+        <v>44013.000000000000</v>
       </c>
       <c r="E5" s="8">
         <v>6758.57</v>
@@ -4479,7 +4479,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="9">
-        <v>44010.000000000000</v>
+        <v>44013.000000000000</v>
       </c>
       <c r="E6" s="8">
         <v>6836.72</v>
@@ -4497,7 +4497,7 @@
         <v>28</v>
       </c>
       <c r="D7" s="9">
-        <v>44010.000000000000</v>
+        <v>44013.000000000000</v>
       </c>
       <c r="E7" s="8">
         <v>4038.64</v>
@@ -4515,7 +4515,7 @@
         <v>28</v>
       </c>
       <c r="D8" s="9">
-        <v>44010.000000000000</v>
+        <v>44013.000000000000</v>
       </c>
       <c r="E8" s="8">
         <v>5746.69</v>
@@ -4533,7 +4533,7 @@
         <v>28</v>
       </c>
       <c r="D9" s="9">
-        <v>44010.000000000000</v>
+        <v>44013.000000000000</v>
       </c>
       <c r="E9" s="8">
         <v>471.62</v>
@@ -4565,7 +4565,7 @@
         <v>25</v>
       </c>
       <c r="D11" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E11" s="8">
         <v>982.68</v>
@@ -4583,7 +4583,7 @@
         <v>25</v>
       </c>
       <c r="D12" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E12" s="8">
         <v>7630.05</v>
@@ -4601,7 +4601,7 @@
         <v>25</v>
       </c>
       <c r="D13" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E13" s="8">
         <v>6001.36</v>
@@ -4619,7 +4619,7 @@
         <v>25</v>
       </c>
       <c r="D14" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E14" s="8">
         <v>8972.09</v>
@@ -4637,7 +4637,7 @@
         <v>25</v>
       </c>
       <c r="D15" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E15" s="8">
         <v>847.44</v>
@@ -4669,7 +4669,7 @@
         <v>27</v>
       </c>
       <c r="D17" s="9">
-        <v>44011.000000000000</v>
+        <v>44014.000000000000</v>
       </c>
       <c r="E17" s="8">
         <v>9950.90</v>
@@ -4687,7 +4687,7 @@
         <v>27</v>
       </c>
       <c r="D18" s="9">
-        <v>44011.000000000000</v>
+        <v>44014.000000000000</v>
       </c>
       <c r="E18" s="8">
         <v>214.52</v>
@@ -4705,7 +4705,7 @@
         <v>27</v>
       </c>
       <c r="D19" s="9">
-        <v>44011.000000000000</v>
+        <v>44014.000000000000</v>
       </c>
       <c r="E19" s="8">
         <v>6220.04</v>
@@ -4737,7 +4737,7 @@
         <v>26</v>
       </c>
       <c r="D21" s="9">
-        <v>44012.000000000000</v>
+        <v>44015.000000000000</v>
       </c>
       <c r="E21" s="8">
         <v>153.90</v>
@@ -4755,7 +4755,7 @@
         <v>26</v>
       </c>
       <c r="D22" s="9">
-        <v>44012.000000000000</v>
+        <v>44015.000000000000</v>
       </c>
       <c r="E22" s="8">
         <v>4164.85</v>
@@ -4848,7 +4848,7 @@
         <v>28</v>
       </c>
       <c r="C4" s="9">
-        <v>44010.000000000000</v>
+        <v>44013.000000000000</v>
       </c>
       <c r="D4" s="8">
         <v>6758.57</v>
@@ -4865,7 +4865,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="D5" s="8">
         <v>982.68</v>
@@ -4882,7 +4882,7 @@
         <v>28</v>
       </c>
       <c r="C6" s="9">
-        <v>44010.000000000000</v>
+        <v>44013.000000000000</v>
       </c>
       <c r="D6" s="8">
         <v>6836.72</v>
@@ -4899,7 +4899,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="9">
-        <v>44010.000000000000</v>
+        <v>44013.000000000000</v>
       </c>
       <c r="D7" s="8">
         <v>4038.64</v>
@@ -4916,7 +4916,7 @@
         <v>25</v>
       </c>
       <c r="C8" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="D8" s="8">
         <v>7630.05</v>
@@ -4933,7 +4933,7 @@
         <v>28</v>
       </c>
       <c r="C9" s="9">
-        <v>44010.000000000000</v>
+        <v>44013.000000000000</v>
       </c>
       <c r="D9" s="8">
         <v>5746.69</v>
@@ -4950,7 +4950,7 @@
         <v>28</v>
       </c>
       <c r="C10" s="9">
-        <v>44010.000000000000</v>
+        <v>44013.000000000000</v>
       </c>
       <c r="D10" s="8">
         <v>471.62</v>
@@ -4967,7 +4967,7 @@
         <v>25</v>
       </c>
       <c r="C11" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="D11" s="8">
         <v>6001.36</v>
@@ -4984,7 +4984,7 @@
         <v>27</v>
       </c>
       <c r="C12" s="9">
-        <v>44011.000000000000</v>
+        <v>44014.000000000000</v>
       </c>
       <c r="D12" s="8">
         <v>9950.90</v>
@@ -5001,7 +5001,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="9">
-        <v>44012.000000000000</v>
+        <v>44015.000000000000</v>
       </c>
       <c r="D13" s="8">
         <v>153.90</v>
@@ -5018,7 +5018,7 @@
         <v>25</v>
       </c>
       <c r="C14" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="D14" s="8">
         <v>8972.09</v>
@@ -5035,7 +5035,7 @@
         <v>27</v>
       </c>
       <c r="C15" s="9">
-        <v>44011.000000000000</v>
+        <v>44014.000000000000</v>
       </c>
       <c r="D15" s="8">
         <v>214.52</v>
@@ -5052,7 +5052,7 @@
         <v>26</v>
       </c>
       <c r="C16" s="9">
-        <v>44012.000000000000</v>
+        <v>44015.000000000000</v>
       </c>
       <c r="D16" s="8">
         <v>4164.85</v>
@@ -5069,7 +5069,7 @@
         <v>25</v>
       </c>
       <c r="C17" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="D17" s="8">
         <v>847.44</v>
@@ -5086,7 +5086,7 @@
         <v>27</v>
       </c>
       <c r="C18" s="9">
-        <v>44011.000000000000</v>
+        <v>44014.000000000000</v>
       </c>
       <c r="D18" s="8">
         <v>6220.04</v>

</xml_diff>

<commit_message>
header lines for Nurbolat
</commit_message>
<xml_diff>
--- a/xtt_demo/02-01_R.xlsx
+++ b/xtt_demo/02-01_R.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\MoldaB\AppData\Local\SAP\SAP GUI\tmp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moldab\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8460" tabRatio="800"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8460" tabRatio="703"/>
   </bookViews>
   <sheets>
     <sheet name="NoGroup" sheetId="2" r:id="rId1"/>
@@ -40,17 +40,18 @@
     <definedName name="F_8">'SimpleTree'!$F$12</definedName>
     <definedName name="F_9">'SimpleTree'!$F$13</definedName>
     <definedName name="RANGE_SUM1">'SimpleTree'!$E$5:$E$19</definedName>
-    <definedName name="_xlnm.Print_Area">'PrintArea (8 rows)'!$A$1:$E$22</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'PrintArea (8 rows)'!$A$1:$E$22</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">NoGroup!$6:$7</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="20" r:id="rId7"/>
+    <pivotCache cacheId="43" r:id="rId7"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>&lt;Caption 1 /&gt;</t>
   </si>
@@ -97,6 +98,9 @@
     <t>&lt;Caption 9 /&gt;</t>
   </si>
   <si>
+    <t>(All)</t>
+  </si>
+  <si>
     <t>01-Jan</t>
   </si>
   <si>
@@ -110,15 +114,6 @@
   </si>
   <si>
     <t>Caption</t>
-  </si>
-  <si>
-    <t>Column Labels</t>
-  </si>
-  <si>
-    <t>Count of SUM 1</t>
-  </si>
-  <si>
-    <t>Count of SUM 2</t>
   </si>
   <si>
     <t>Date</t>
@@ -145,19 +140,19 @@
     <t>Group</t>
   </si>
   <si>
-    <t>Groups</t>
-  </si>
-  <si>
-    <t>Jan</t>
-  </si>
-  <si>
-    <t>Row Labels</t>
+    <t>Months</t>
   </si>
   <si>
     <t>SUM 1</t>
   </si>
   <si>
     <t>SUM 2</t>
+  </si>
+  <si>
+    <t>Sum of SUM 1</t>
+  </si>
+  <si>
+    <t>Sum of SUM 2</t>
   </si>
   <si>
     <t>Sums by group GRP A</t>
@@ -176,12 +171,6 @@
   </si>
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>Total Count of SUM 1</t>
-  </si>
-  <si>
-    <t>Total Count of SUM 2</t>
   </si>
   <si>
     <t>Watch Formula</t>
@@ -787,7 +776,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -869,13 +858,7 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1127,10 +1110,41 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[ZXXT_02_EXCEL.xlsx]Pivot based on ExcelTable!PivotTable1</c:name>
+    <c:name>[ZXXT_02_EXCEL.XLSX]Pivot based on ExcelTable!PivotTable1</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:pivotFmts>
       <c:pivotFmt>
@@ -1208,40 +1222,160 @@
           <c:symbol val="none"/>
         </c:marker>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="12"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Pivot based on ExcelTable'!$B$3:$B$5</c:f>
+              <c:f>'Pivot based on ExcelTable'!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Groups - Count of SUM 1</c:v>
+                  <c:v>Sum of SUM 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-0E2D-4ACA-B2DD-18EF0C7BC1D0}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Pivot based on ExcelTable'!$A$6:$A$8</c:f>
+              <c:f>'Pivot based on ExcelTable'!$A$4:$B$5</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="1"/>
                 <c:lvl>
@@ -1251,7 +1385,7 @@
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>Jan</c:v>
+                    <c:v>Date</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -1259,12 +1393,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pivot based on ExcelTable'!$B$6:$B$8</c:f>
+              <c:f>'Pivot based on ExcelTable'!$C$4:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1280,28 +1414,36 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Pivot based on ExcelTable'!$C$3:$C$5</c:f>
+              <c:f>'Pivot based on ExcelTable'!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Groups - Count of SUM 2</c:v>
+                  <c:v>Sum of SUM 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-0E2D-4ACA-B2DD-18EF0C7BC1D0}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Pivot based on ExcelTable'!$A$6:$A$8</c:f>
+              <c:f>'Pivot based on ExcelTable'!$A$4:$B$5</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="1"/>
                 <c:lvl>
@@ -1311,7 +1453,7 @@
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>Jan</c:v>
+                    <c:v>Date</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -1319,12 +1461,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pivot based on ExcelTable'!$C$6:$C$8</c:f>
+              <c:f>'Pivot based on ExcelTable'!$D$4:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1342,119 +1484,10 @@
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="294297368"/>
-        <c:axId val="294296384"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="294297368"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="294296384"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="294296384"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="294297368"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2127,18 +2160,18 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshOnLoad="1" refreshedBy="Moldabayev, Birzhan" refreshedDate="44013.699615740741" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshOnLoad="1" refreshedBy="Moldabayev, Birzhan" refreshedDate="44019.56553738426" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="Caption" numFmtId="0">
-      <sharedItems/>
+      <sharedItems count="1">
+        <s v="{R-T-CAPTION}"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Group" numFmtId="0">
-      <sharedItems count="1">
-        <s v="{R-T-GROUP}"/>
-      </sharedItems>
+      <sharedItems/>
     </cacheField>
     <cacheField name="Date" numFmtId="14">
       <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2020-01-01T00:00:00" maxDate="2020-01-02T00:00:00" count="1">
@@ -2555,17 +2588,17 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
-  <location ref="A3:E8" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="43" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
+  <location ref="A3:D5" firstHeaderRow="0" firstDataRow="1" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
+    <pivotField axis="axisPage" compact="0" outline="0" showAll="0">
       <items count="2">
-        <item n="Groups" x="0"/>
+        <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
       <items count="369">
         <item x="0"/>
         <item x="1"/>
@@ -2938,12 +2971,12 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="14">
         <item x="0"/>
-        <item x="1"/>
+        <item n="Date" x="1"/>
         <item x="2"/>
         <item x="3"/>
         <item x="4"/>
@@ -2963,61 +2996,48 @@
     <field x="5"/>
     <field x="2"/>
   </rowFields>
-  <rowItems count="3">
+  <rowItems count="2">
     <i>
       <x v="1"/>
-    </i>
-    <i r="1">
       <x v="1"/>
     </i>
     <i t="grand">
       <x/>
     </i>
   </rowItems>
-  <colFields count="2">
-    <field x="1"/>
+  <colFields count="1">
     <field x="-2"/>
   </colFields>
-  <colItems count="4">
+  <colItems count="2">
     <i>
       <x/>
-      <x/>
     </i>
-    <i r="1" i="1">
+    <i i="1">
       <x v="1"/>
     </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
   </colItems>
+  <pageFields count="1">
+    <pageField fld="0" hier="-1"/>
+  </pageFields>
   <dataFields count="2">
-    <dataField name="Count of SUM 1" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="Count of SUM 2" fld="4" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Sum of SUM 1" fld="3" baseField="2" baseItem="0"/>
+    <dataField name="Sum of SUM 2" fld="4" baseField="2" baseItem="0"/>
   </dataFields>
   <chartFormats count="2">
-    <chartFormat chart="0" format="3" series="1">
+    <chartFormat chart="0" format="11" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
+        <references count="1">
           <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="4" series="1">
+    <chartFormat chart="0" format="12" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
+        <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="1"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
@@ -3343,10 +3363,341 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col customWidth="1" hidden="1" max="1" min="1" outlineLevel="1" width="20.7109375"/>
+    <col collapsed="1" customWidth="1" max="2" min="2" width="40.28515625"/>
+    <col customWidth="1" max="3" min="3" width="35.42578125"/>
+    <col customWidth="1" max="4" min="4" width="14.85546875"/>
+    <col customWidth="1" max="5" min="5" width="33.42578125"/>
+    <col customWidth="1" max="6" min="6" width="33.42578125"/>
+  </cols>
+  <sheetData>
+    <row r="1" hidden="1" outlineLevel="1">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" hidden="1" outlineLevel="1">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" hidden="1" outlineLevel="1">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" hidden="1" outlineLevel="1">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="9">
+        <v>44016.000000000000</v>
+      </c>
+      <c r="E8" s="8">
+        <v>6758.57</v>
+      </c>
+      <c r="F8" s="8">
+        <v>5563.86</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="9">
+        <v>44019.000000000000</v>
+      </c>
+      <c r="E9" s="8">
+        <v>982.68</v>
+      </c>
+      <c r="F9" s="8">
+        <v>9927.07</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="9">
+        <v>44016.000000000000</v>
+      </c>
+      <c r="E10" s="8">
+        <v>6836.72</v>
+      </c>
+      <c r="F10" s="8">
+        <v>7795.09</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="9">
+        <v>44016.000000000000</v>
+      </c>
+      <c r="E11" s="8">
+        <v>4038.64</v>
+      </c>
+      <c r="F11" s="8">
+        <v>7742.85</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="9">
+        <v>44019.000000000000</v>
+      </c>
+      <c r="E12" s="8">
+        <v>7630.05</v>
+      </c>
+      <c r="F12" s="8">
+        <v>6014.38</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="9">
+        <v>44016.000000000000</v>
+      </c>
+      <c r="E13" s="8">
+        <v>5746.69</v>
+      </c>
+      <c r="F13" s="8">
+        <v>1997.34</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="9">
+        <v>44016.000000000000</v>
+      </c>
+      <c r="E14" s="8">
+        <v>471.62</v>
+      </c>
+      <c r="F14" s="8">
+        <v>6510.54</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="9">
+        <v>44019.000000000000</v>
+      </c>
+      <c r="E15" s="8">
+        <v>6001.36</v>
+      </c>
+      <c r="F15" s="8">
+        <v>7509.60</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="9">
+        <v>44017.000000000000</v>
+      </c>
+      <c r="E16" s="8">
+        <v>9950.90</v>
+      </c>
+      <c r="F16" s="8">
+        <v>7487.59</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="9">
+        <v>44018.000000000000</v>
+      </c>
+      <c r="E17" s="8">
+        <v>153.90</v>
+      </c>
+      <c r="F17" s="8">
+        <v>7473.27</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="9">
+        <v>44019.000000000000</v>
+      </c>
+      <c r="E18" s="8">
+        <v>8972.09</v>
+      </c>
+      <c r="F18" s="8">
+        <v>1796.79</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="9">
+        <v>44017.000000000000</v>
+      </c>
+      <c r="E19" s="8">
+        <v>214.52</v>
+      </c>
+      <c r="F19" s="8">
+        <v>8481.91</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="9">
+        <v>44018.000000000000</v>
+      </c>
+      <c r="E20" s="8">
+        <v>4164.85</v>
+      </c>
+      <c r="F20" s="8">
+        <v>4263.78</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="9">
+        <v>44019.000000000000</v>
+      </c>
+      <c r="E21" s="8">
+        <v>847.44</v>
+      </c>
+      <c r="F21" s="8">
+        <v>1515.22</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="9">
+        <v>44017.000000000000</v>
+      </c>
+      <c r="E22" s="8">
+        <v>6220.04</v>
+      </c>
+      <c r="F22" s="8">
+        <v>6482.36</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C22">
+      <formula1>$A$1:$A$4</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="85" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3361,335 +3712,29 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="23" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2">
       <c r="B2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="9">
-        <v>44013.000000000000</v>
-      </c>
-      <c r="E5" s="8">
-        <v>6758.57</v>
-      </c>
-      <c r="F5" s="8">
-        <v>5563.86</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="9">
-        <v>44016.000000000000</v>
-      </c>
-      <c r="E6" s="8">
-        <v>982.68</v>
-      </c>
-      <c r="F6" s="8">
-        <v>9927.07</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="9">
-        <v>44013.000000000000</v>
-      </c>
-      <c r="E7" s="8">
-        <v>6836.72</v>
-      </c>
-      <c r="F7" s="8">
-        <v>7795.09</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="9">
-        <v>44013.000000000000</v>
-      </c>
-      <c r="E8" s="8">
-        <v>4038.64</v>
-      </c>
-      <c r="F8" s="8">
-        <v>7742.85</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="9">
-        <v>44016.000000000000</v>
-      </c>
-      <c r="E9" s="8">
-        <v>7630.05</v>
-      </c>
-      <c r="F9" s="8">
-        <v>6014.38</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="9">
-        <v>44013.000000000000</v>
-      </c>
-      <c r="E10" s="8">
-        <v>5746.69</v>
-      </c>
-      <c r="F10" s="8">
-        <v>1997.34</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="9">
-        <v>44013.000000000000</v>
-      </c>
-      <c r="E11" s="8">
-        <v>471.62</v>
-      </c>
-      <c r="F11" s="8">
-        <v>6510.54</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="9">
-        <v>44016.000000000000</v>
-      </c>
-      <c r="E12" s="8">
-        <v>6001.36</v>
-      </c>
-      <c r="F12" s="8">
-        <v>7509.60</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="9">
-        <v>44014.000000000000</v>
-      </c>
-      <c r="E13" s="8">
-        <v>9950.90</v>
-      </c>
-      <c r="F13" s="8">
-        <v>7487.59</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="9">
-        <v>44015.000000000000</v>
-      </c>
-      <c r="E14" s="8">
-        <v>153.90</v>
-      </c>
-      <c r="F14" s="8">
-        <v>7473.27</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="9">
-        <v>44016.000000000000</v>
-      </c>
-      <c r="E15" s="8">
-        <v>8972.09</v>
-      </c>
-      <c r="F15" s="8">
-        <v>1796.79</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="9">
-        <v>44014.000000000000</v>
-      </c>
-      <c r="E16" s="8">
-        <v>214.52</v>
-      </c>
-      <c r="F16" s="8">
-        <v>8481.91</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="9">
-        <v>44015.000000000000</v>
-      </c>
-      <c r="E17" s="8">
-        <v>4164.85</v>
-      </c>
-      <c r="F17" s="8">
-        <v>4263.78</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="9">
-        <v>44016.000000000000</v>
-      </c>
-      <c r="E18" s="8">
-        <v>847.44</v>
-      </c>
-      <c r="F18" s="8">
-        <v>1515.22</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="9">
-        <v>44014.000000000000</v>
-      </c>
-      <c r="E19" s="8">
-        <v>6220.04</v>
-      </c>
-      <c r="F19" s="8">
-        <v>6482.36</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col customWidth="1" max="1" min="1" width="20.7109375"/>
-    <col customWidth="1" max="2" min="2" width="40.28515625"/>
-    <col customWidth="1" max="3" min="3" width="35.42578125"/>
-    <col customWidth="1" max="4" min="4" width="14.85546875"/>
-    <col customWidth="1" max="5" min="5" width="33.42578125"/>
-    <col customWidth="1" max="6" min="6" width="33.42578125"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="B2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>34</v>
-      </c>
       <c r="F4" s="10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5">
@@ -3697,10 +3742,10 @@
         <v>0</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D5" s="13">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E5" s="14">
         <v>6758.57</v>
@@ -3714,10 +3759,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6" s="13">
-        <v>44016.000000000000</v>
+        <v>44019.000000000000</v>
       </c>
       <c r="E6" s="14">
         <v>982.68</v>
@@ -3731,10 +3776,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7" s="13">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E7" s="14">
         <v>6836.72</v>
@@ -3748,10 +3793,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8" s="13">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E8" s="14">
         <v>4038.64</v>
@@ -3765,10 +3810,10 @@
         <v>10</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" s="13">
-        <v>44016.000000000000</v>
+        <v>44019.000000000000</v>
       </c>
       <c r="E9" s="14">
         <v>7630.05</v>
@@ -3782,10 +3827,10 @@
         <v>11</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D10" s="13">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E10" s="14">
         <v>5746.69</v>
@@ -3799,10 +3844,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D11" s="13">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E11" s="14">
         <v>471.62</v>
@@ -3816,10 +3861,10 @@
         <v>13</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" s="13">
-        <v>44016.000000000000</v>
+        <v>44019.000000000000</v>
       </c>
       <c r="E12" s="14">
         <v>6001.36</v>
@@ -3833,10 +3878,10 @@
         <v>14</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D13" s="13">
-        <v>44014.000000000000</v>
+        <v>44017.000000000000</v>
       </c>
       <c r="E13" s="14">
         <v>9950.90</v>
@@ -3850,10 +3895,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D14" s="13">
-        <v>44015.000000000000</v>
+        <v>44018.000000000000</v>
       </c>
       <c r="E14" s="14">
         <v>153.90</v>
@@ -3867,10 +3912,10 @@
         <v>2</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D15" s="13">
-        <v>44016.000000000000</v>
+        <v>44019.000000000000</v>
       </c>
       <c r="E15" s="14">
         <v>8972.09</v>
@@ -3884,10 +3929,10 @@
         <v>3</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D16" s="13">
-        <v>44014.000000000000</v>
+        <v>44017.000000000000</v>
       </c>
       <c r="E16" s="14">
         <v>214.52</v>
@@ -3901,10 +3946,10 @@
         <v>4</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D17" s="13">
-        <v>44015.000000000000</v>
+        <v>44018.000000000000</v>
       </c>
       <c r="E17" s="14">
         <v>4164.85</v>
@@ -3918,10 +3963,10 @@
         <v>5</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D18" s="13">
-        <v>44016.000000000000</v>
+        <v>44019.000000000000</v>
       </c>
       <c r="E18" s="14">
         <v>847.44</v>
@@ -3935,10 +3980,10 @@
         <v>6</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D19" s="13">
-        <v>44014.000000000000</v>
+        <v>44017.000000000000</v>
       </c>
       <c r="E19" s="14">
         <v>6220.04</v>
@@ -3949,7 +3994,7 @@
     </row>
     <row r="20">
       <c r="B20" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="15"/>
@@ -3971,89 +4016,65 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E8"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="13.140625"/>
-    <col customWidth="1" max="2" min="2" width="16.28515625"/>
-    <col customWidth="1" max="3" min="3" width="14.85546875"/>
-    <col customWidth="1" max="4" min="4" width="19.85546875"/>
-    <col customWidth="1" max="5" min="5" width="19.85546875"/>
+    <col customWidth="1" max="1" min="1" width="11.28515625"/>
+    <col customWidth="1" max="2" min="2" width="7.42578125"/>
+    <col customWidth="1" max="3" min="3" width="13.42578125"/>
+    <col customWidth="1" max="4" min="4" width="13.42578125"/>
   </cols>
   <sheetData>
+    <row r="1">
+      <c r="A1" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="3">
+      <c r="A3" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="B3" s="32" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
       <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" t="s">
-        <v>43</v>
+        <v>16</v>
+      </c>
+      <c r="C4" s="33">
+        <v>0</v>
+      </c>
+      <c r="D4" s="33">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="34">
-        <v>1</v>
-      </c>
-      <c r="C7" s="34">
-        <v>1</v>
-      </c>
-      <c r="D7" s="34">
-        <v>1</v>
-      </c>
-      <c r="E7" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="34">
-        <v>1</v>
-      </c>
-      <c r="C8" s="34">
-        <v>1</v>
-      </c>
-      <c r="D8" s="34">
-        <v>1</v>
-      </c>
-      <c r="E8" s="34">
-        <v>1</v>
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="33">
+        <v>0</v>
+      </c>
+      <c r="D5" s="33">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4085,24 +4106,24 @@
     </row>
     <row r="2">
       <c r="B2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="F4" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5">
@@ -4111,10 +4132,10 @@
         <v>0</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D5" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E5" s="8">
         <v>6758.57</v>
@@ -4129,10 +4150,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6" s="9">
-        <v>44016.000000000000</v>
+        <v>44019.000000000000</v>
       </c>
       <c r="E6" s="8">
         <v>982.68</v>
@@ -4147,10 +4168,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E7" s="8">
         <v>6836.72</v>
@@ -4165,10 +4186,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E8" s="8">
         <v>4038.64</v>
@@ -4183,10 +4204,10 @@
         <v>10</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" s="9">
-        <v>44016.000000000000</v>
+        <v>44019.000000000000</v>
       </c>
       <c r="E9" s="8">
         <v>7630.05</v>
@@ -4201,10 +4222,10 @@
         <v>11</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D10" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E10" s="8">
         <v>5746.69</v>
@@ -4219,10 +4240,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D11" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E11" s="8">
         <v>471.62</v>
@@ -4237,10 +4258,10 @@
         <v>13</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" s="9">
-        <v>44016.000000000000</v>
+        <v>44019.000000000000</v>
       </c>
       <c r="E12" s="8">
         <v>6001.36</v>
@@ -4255,10 +4276,10 @@
         <v>14</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D13" s="9">
-        <v>44014.000000000000</v>
+        <v>44017.000000000000</v>
       </c>
       <c r="E13" s="8">
         <v>9950.90</v>
@@ -4273,10 +4294,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D14" s="9">
-        <v>44015.000000000000</v>
+        <v>44018.000000000000</v>
       </c>
       <c r="E14" s="8">
         <v>153.90</v>
@@ -4291,10 +4312,10 @@
         <v>2</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D15" s="9">
-        <v>44016.000000000000</v>
+        <v>44019.000000000000</v>
       </c>
       <c r="E15" s="8">
         <v>8972.09</v>
@@ -4309,10 +4330,10 @@
         <v>3</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D16" s="9">
-        <v>44014.000000000000</v>
+        <v>44017.000000000000</v>
       </c>
       <c r="E16" s="8">
         <v>214.52</v>
@@ -4327,10 +4348,10 @@
         <v>4</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D17" s="9">
-        <v>44015.000000000000</v>
+        <v>44018.000000000000</v>
       </c>
       <c r="E17" s="8">
         <v>4164.85</v>
@@ -4345,10 +4366,10 @@
         <v>5</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D18" s="9">
-        <v>44016.000000000000</v>
+        <v>44019.000000000000</v>
       </c>
       <c r="E18" s="8">
         <v>847.44</v>
@@ -4363,10 +4384,10 @@
         <v>6</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D19" s="9">
-        <v>44014.000000000000</v>
+        <v>44017.000000000000</v>
       </c>
       <c r="E19" s="8">
         <v>6220.04</v>
@@ -4378,11 +4399,11 @@
     <row r="20">
       <c r="A20" t="s"/>
       <c r="B20" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E20" s="18">
         <v>68990.07</v>
@@ -4394,7 +4415,7 @@
     <row r="21">
       <c r="A21" t="s"/>
       <c r="D21" s="20" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E21" s="22">
         <f>SUM(RANGE_SUM1)</f>
@@ -4432,24 +4453,24 @@
     </row>
     <row r="2">
       <c r="B2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="F4" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" hidden="1" outlineLevel="1">
@@ -4458,10 +4479,10 @@
         <v>0</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D5" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E5" s="8">
         <v>6758.57</v>
@@ -4476,10 +4497,10 @@
         <v>8</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D6" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E6" s="8">
         <v>6836.72</v>
@@ -4494,10 +4515,10 @@
         <v>9</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E7" s="8">
         <v>4038.64</v>
@@ -4512,10 +4533,10 @@
         <v>11</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E8" s="8">
         <v>5746.69</v>
@@ -4530,10 +4551,10 @@
         <v>12</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D9" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="E9" s="8">
         <v>471.62</v>
@@ -4545,7 +4566,7 @@
     <row r="10">
       <c r="A10" t="s"/>
       <c r="B10" s="24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C10" s="25"/>
       <c r="D10" s="26"/>
@@ -4562,10 +4583,10 @@
         <v>7</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D11" s="9">
-        <v>44016.000000000000</v>
+        <v>44019.000000000000</v>
       </c>
       <c r="E11" s="8">
         <v>982.68</v>
@@ -4580,10 +4601,10 @@
         <v>10</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" s="9">
-        <v>44016.000000000000</v>
+        <v>44019.000000000000</v>
       </c>
       <c r="E12" s="8">
         <v>7630.05</v>
@@ -4598,10 +4619,10 @@
         <v>13</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D13" s="9">
-        <v>44016.000000000000</v>
+        <v>44019.000000000000</v>
       </c>
       <c r="E13" s="8">
         <v>6001.36</v>
@@ -4616,10 +4637,10 @@
         <v>2</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D14" s="9">
-        <v>44016.000000000000</v>
+        <v>44019.000000000000</v>
       </c>
       <c r="E14" s="8">
         <v>8972.09</v>
@@ -4634,10 +4655,10 @@
         <v>5</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D15" s="9">
-        <v>44016.000000000000</v>
+        <v>44019.000000000000</v>
       </c>
       <c r="E15" s="8">
         <v>847.44</v>
@@ -4649,7 +4670,7 @@
     <row r="16">
       <c r="A16" t="s"/>
       <c r="B16" s="24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C16" s="25"/>
       <c r="D16" s="26"/>
@@ -4666,10 +4687,10 @@
         <v>14</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D17" s="9">
-        <v>44014.000000000000</v>
+        <v>44017.000000000000</v>
       </c>
       <c r="E17" s="8">
         <v>9950.90</v>
@@ -4684,10 +4705,10 @@
         <v>3</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D18" s="9">
-        <v>44014.000000000000</v>
+        <v>44017.000000000000</v>
       </c>
       <c r="E18" s="8">
         <v>214.52</v>
@@ -4702,10 +4723,10 @@
         <v>6</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D19" s="9">
-        <v>44014.000000000000</v>
+        <v>44017.000000000000</v>
       </c>
       <c r="E19" s="8">
         <v>6220.04</v>
@@ -4717,7 +4738,7 @@
     <row r="20">
       <c r="A20" t="s"/>
       <c r="B20" s="24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C20" s="25"/>
       <c r="D20" s="26"/>
@@ -4734,10 +4755,10 @@
         <v>1</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D21" s="9">
-        <v>44015.000000000000</v>
+        <v>44018.000000000000</v>
       </c>
       <c r="E21" s="8">
         <v>153.90</v>
@@ -4752,10 +4773,10 @@
         <v>4</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D22" s="9">
-        <v>44015.000000000000</v>
+        <v>44018.000000000000</v>
       </c>
       <c r="E22" s="8">
         <v>4164.85</v>
@@ -4767,7 +4788,7 @@
     <row r="23">
       <c r="A23" t="s"/>
       <c r="B23" s="24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C23" s="25"/>
       <c r="D23" s="26"/>
@@ -4781,7 +4802,7 @@
     <row r="24">
       <c r="A24" t="s"/>
       <c r="B24" s="28" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C24" s="29"/>
       <c r="D24" s="30"/>
@@ -4820,24 +4841,24 @@
     </row>
     <row r="2" customHeight="1" ht="15.75">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" customHeight="1" ht="15">
       <c r="A3" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E3" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" customHeight="1" ht="15">
@@ -4845,10 +4866,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="D4" s="8">
         <v>6758.57</v>
@@ -4862,10 +4883,10 @@
         <v>7</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" s="9">
-        <v>44016.000000000000</v>
+        <v>44019.000000000000</v>
       </c>
       <c r="D5" s="8">
         <v>982.68</v>
@@ -4879,10 +4900,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C6" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="D6" s="8">
         <v>6836.72</v>
@@ -4896,10 +4917,10 @@
         <v>9</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="D7" s="8">
         <v>4038.64</v>
@@ -4913,10 +4934,10 @@
         <v>10</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" s="9">
-        <v>44016.000000000000</v>
+        <v>44019.000000000000</v>
       </c>
       <c r="D8" s="8">
         <v>7630.05</v>
@@ -4930,10 +4951,10 @@
         <v>11</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C9" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="D9" s="8">
         <v>5746.69</v>
@@ -4947,10 +4968,10 @@
         <v>12</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10" s="9">
-        <v>44013.000000000000</v>
+        <v>44016.000000000000</v>
       </c>
       <c r="D10" s="8">
         <v>471.62</v>
@@ -4964,10 +4985,10 @@
         <v>13</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11" s="9">
-        <v>44016.000000000000</v>
+        <v>44019.000000000000</v>
       </c>
       <c r="D11" s="8">
         <v>6001.36</v>
@@ -4981,10 +5002,10 @@
         <v>14</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" s="9">
-        <v>44014.000000000000</v>
+        <v>44017.000000000000</v>
       </c>
       <c r="D12" s="8">
         <v>9950.90</v>
@@ -4998,10 +5019,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C13" s="9">
-        <v>44015.000000000000</v>
+        <v>44018.000000000000</v>
       </c>
       <c r="D13" s="8">
         <v>153.90</v>
@@ -5015,10 +5036,10 @@
         <v>2</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" s="9">
-        <v>44016.000000000000</v>
+        <v>44019.000000000000</v>
       </c>
       <c r="D14" s="8">
         <v>8972.09</v>
@@ -5032,10 +5053,10 @@
         <v>3</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" s="9">
-        <v>44014.000000000000</v>
+        <v>44017.000000000000</v>
       </c>
       <c r="D15" s="8">
         <v>214.52</v>
@@ -5049,10 +5070,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C16" s="9">
-        <v>44015.000000000000</v>
+        <v>44018.000000000000</v>
       </c>
       <c r="D16" s="8">
         <v>4164.85</v>
@@ -5066,10 +5087,10 @@
         <v>5</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C17" s="9">
-        <v>44016.000000000000</v>
+        <v>44019.000000000000</v>
       </c>
       <c r="D17" s="8">
         <v>847.44</v>
@@ -5083,10 +5104,10 @@
         <v>6</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C18" s="9">
-        <v>44014.000000000000</v>
+        <v>44017.000000000000</v>
       </c>
       <c r="D18" s="8">
         <v>6220.04</v>
@@ -5097,7 +5118,7 @@
     </row>
     <row r="22" customHeight="1" ht="15">
       <c r="E22" s="21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix empty cell for drawing
</commit_message>
<xml_diff>
--- a/xtt_demo/02-01_R.xlsx
+++ b/xtt_demo/02-01_R.xlsx
@@ -3434,7 +3434,7 @@
         <v>26</v>
       </c>
       <c r="D8" s="9">
-        <v>44066.000000000000</v>
+        <v>44067.000000000000</v>
       </c>
       <c r="E8" s="8">
         <v>6758.57</v>
@@ -3451,7 +3451,7 @@
         <v>23</v>
       </c>
       <c r="D9" s="9">
-        <v>44069.000000000000</v>
+        <v>44070.000000000000</v>
       </c>
       <c r="E9" s="8">
         <v>982.68</v>
@@ -3468,7 +3468,7 @@
         <v>26</v>
       </c>
       <c r="D10" s="9">
-        <v>44066.000000000000</v>
+        <v>44067.000000000000</v>
       </c>
       <c r="E10" s="8">
         <v>6836.72</v>
@@ -3485,7 +3485,7 @@
         <v>26</v>
       </c>
       <c r="D11" s="9">
-        <v>44066.000000000000</v>
+        <v>44067.000000000000</v>
       </c>
       <c r="E11" s="8">
         <v>4038.64</v>
@@ -3502,7 +3502,7 @@
         <v>23</v>
       </c>
       <c r="D12" s="9">
-        <v>44069.000000000000</v>
+        <v>44070.000000000000</v>
       </c>
       <c r="E12" s="8">
         <v>7630.05</v>
@@ -3519,7 +3519,7 @@
         <v>26</v>
       </c>
       <c r="D13" s="9">
-        <v>44066.000000000000</v>
+        <v>44067.000000000000</v>
       </c>
       <c r="E13" s="8">
         <v>5746.69</v>
@@ -3536,7 +3536,7 @@
         <v>26</v>
       </c>
       <c r="D14" s="9">
-        <v>44066.000000000000</v>
+        <v>44067.000000000000</v>
       </c>
       <c r="E14" s="8">
         <v>471.62</v>
@@ -3553,7 +3553,7 @@
         <v>23</v>
       </c>
       <c r="D15" s="9">
-        <v>44069.000000000000</v>
+        <v>44070.000000000000</v>
       </c>
       <c r="E15" s="8">
         <v>6001.36</v>
@@ -3570,7 +3570,7 @@
         <v>25</v>
       </c>
       <c r="D16" s="9">
-        <v>44067.000000000000</v>
+        <v>44068.000000000000</v>
       </c>
       <c r="E16" s="8">
         <v>9950.90</v>
@@ -3587,7 +3587,7 @@
         <v>24</v>
       </c>
       <c r="D17" s="9">
-        <v>44068.000000000000</v>
+        <v>44069.000000000000</v>
       </c>
       <c r="E17" s="8">
         <v>153.90</v>
@@ -3604,7 +3604,7 @@
         <v>23</v>
       </c>
       <c r="D18" s="9">
-        <v>44069.000000000000</v>
+        <v>44070.000000000000</v>
       </c>
       <c r="E18" s="8">
         <v>8972.09</v>
@@ -3621,7 +3621,7 @@
         <v>25</v>
       </c>
       <c r="D19" s="9">
-        <v>44067.000000000000</v>
+        <v>44068.000000000000</v>
       </c>
       <c r="E19" s="8">
         <v>214.52</v>
@@ -3638,7 +3638,7 @@
         <v>24</v>
       </c>
       <c r="D20" s="9">
-        <v>44068.000000000000</v>
+        <v>44069.000000000000</v>
       </c>
       <c r="E20" s="8">
         <v>4164.85</v>
@@ -3655,7 +3655,7 @@
         <v>23</v>
       </c>
       <c r="D21" s="9">
-        <v>44069.000000000000</v>
+        <v>44070.000000000000</v>
       </c>
       <c r="E21" s="8">
         <v>847.44</v>
@@ -3672,7 +3672,7 @@
         <v>25</v>
       </c>
       <c r="D22" s="9">
-        <v>44067.000000000000</v>
+        <v>44068.000000000000</v>
       </c>
       <c r="E22" s="8">
         <v>6220.04</v>
@@ -3745,7 +3745,7 @@
         <v>26</v>
       </c>
       <c r="D5" s="13">
-        <v>44066.000000000000</v>
+        <v>44067.000000000000</v>
       </c>
       <c r="E5" s="14">
         <v>6758.57</v>
@@ -3762,7 +3762,7 @@
         <v>23</v>
       </c>
       <c r="D6" s="13">
-        <v>44069.000000000000</v>
+        <v>44070.000000000000</v>
       </c>
       <c r="E6" s="14">
         <v>982.68</v>
@@ -3779,7 +3779,7 @@
         <v>26</v>
       </c>
       <c r="D7" s="13">
-        <v>44066.000000000000</v>
+        <v>44067.000000000000</v>
       </c>
       <c r="E7" s="14">
         <v>6836.72</v>
@@ -3796,7 +3796,7 @@
         <v>26</v>
       </c>
       <c r="D8" s="13">
-        <v>44066.000000000000</v>
+        <v>44067.000000000000</v>
       </c>
       <c r="E8" s="14">
         <v>4038.64</v>
@@ -3813,7 +3813,7 @@
         <v>23</v>
       </c>
       <c r="D9" s="13">
-        <v>44069.000000000000</v>
+        <v>44070.000000000000</v>
       </c>
       <c r="E9" s="14">
         <v>7630.05</v>
@@ -3830,7 +3830,7 @@
         <v>26</v>
       </c>
       <c r="D10" s="13">
-        <v>44066.000000000000</v>
+        <v>44067.000000000000</v>
       </c>
       <c r="E10" s="14">
         <v>5746.69</v>
@@ -3847,7 +3847,7 @@
         <v>26</v>
       </c>
       <c r="D11" s="13">
-        <v>44066.000000000000</v>
+        <v>44067.000000000000</v>
       </c>
       <c r="E11" s="14">
         <v>471.62</v>
@@ -3864,7 +3864,7 @@
         <v>23</v>
       </c>
       <c r="D12" s="13">
-        <v>44069.000000000000</v>
+        <v>44070.000000000000</v>
       </c>
       <c r="E12" s="14">
         <v>6001.36</v>
@@ -3881,7 +3881,7 @@
         <v>25</v>
       </c>
       <c r="D13" s="13">
-        <v>44067.000000000000</v>
+        <v>44068.000000000000</v>
       </c>
       <c r="E13" s="14">
         <v>9950.90</v>
@@ -3898,7 +3898,7 @@
         <v>24</v>
       </c>
       <c r="D14" s="13">
-        <v>44068.000000000000</v>
+        <v>44069.000000000000</v>
       </c>
       <c r="E14" s="14">
         <v>153.90</v>
@@ -3915,7 +3915,7 @@
         <v>23</v>
       </c>
       <c r="D15" s="13">
-        <v>44069.000000000000</v>
+        <v>44070.000000000000</v>
       </c>
       <c r="E15" s="14">
         <v>8972.09</v>
@@ -3932,7 +3932,7 @@
         <v>25</v>
       </c>
       <c r="D16" s="13">
-        <v>44067.000000000000</v>
+        <v>44068.000000000000</v>
       </c>
       <c r="E16" s="14">
         <v>214.52</v>
@@ -3949,7 +3949,7 @@
         <v>24</v>
       </c>
       <c r="D17" s="13">
-        <v>44068.000000000000</v>
+        <v>44069.000000000000</v>
       </c>
       <c r="E17" s="14">
         <v>4164.85</v>
@@ -3966,7 +3966,7 @@
         <v>23</v>
       </c>
       <c r="D18" s="13">
-        <v>44069.000000000000</v>
+        <v>44070.000000000000</v>
       </c>
       <c r="E18" s="14">
         <v>847.44</v>
@@ -3983,7 +3983,7 @@
         <v>25</v>
       </c>
       <c r="D19" s="13">
-        <v>44067.000000000000</v>
+        <v>44068.000000000000</v>
       </c>
       <c r="E19" s="14">
         <v>6220.04</v>
@@ -4004,7 +4004,6 @@
       <c r="F20" s="14">
         <f>SUBTOTAL(109,Table1[SUM 2])</f>
       </c>
-      <c r="F20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4077,7 +4076,6 @@
       <c r="D5" s="33">
         <v>0</v>
       </c>
-      <c r="D5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4137,7 +4135,7 @@
         <v>26</v>
       </c>
       <c r="D5" s="9">
-        <v>44066.000000000000</v>
+        <v>44067.000000000000</v>
       </c>
       <c r="E5" s="8">
         <v>6758.57</v>
@@ -4155,7 +4153,7 @@
         <v>23</v>
       </c>
       <c r="D6" s="9">
-        <v>44069.000000000000</v>
+        <v>44070.000000000000</v>
       </c>
       <c r="E6" s="8">
         <v>982.68</v>
@@ -4173,7 +4171,7 @@
         <v>26</v>
       </c>
       <c r="D7" s="9">
-        <v>44066.000000000000</v>
+        <v>44067.000000000000</v>
       </c>
       <c r="E7" s="8">
         <v>6836.72</v>
@@ -4191,7 +4189,7 @@
         <v>26</v>
       </c>
       <c r="D8" s="9">
-        <v>44066.000000000000</v>
+        <v>44067.000000000000</v>
       </c>
       <c r="E8" s="8">
         <v>4038.64</v>
@@ -4209,7 +4207,7 @@
         <v>23</v>
       </c>
       <c r="D9" s="9">
-        <v>44069.000000000000</v>
+        <v>44070.000000000000</v>
       </c>
       <c r="E9" s="8">
         <v>7630.05</v>
@@ -4227,7 +4225,7 @@
         <v>26</v>
       </c>
       <c r="D10" s="9">
-        <v>44066.000000000000</v>
+        <v>44067.000000000000</v>
       </c>
       <c r="E10" s="8">
         <v>5746.69</v>
@@ -4245,7 +4243,7 @@
         <v>26</v>
       </c>
       <c r="D11" s="9">
-        <v>44066.000000000000</v>
+        <v>44067.000000000000</v>
       </c>
       <c r="E11" s="8">
         <v>471.62</v>
@@ -4263,7 +4261,7 @@
         <v>23</v>
       </c>
       <c r="D12" s="9">
-        <v>44069.000000000000</v>
+        <v>44070.000000000000</v>
       </c>
       <c r="E12" s="8">
         <v>6001.36</v>
@@ -4281,7 +4279,7 @@
         <v>25</v>
       </c>
       <c r="D13" s="9">
-        <v>44067.000000000000</v>
+        <v>44068.000000000000</v>
       </c>
       <c r="E13" s="8">
         <v>9950.90</v>
@@ -4299,7 +4297,7 @@
         <v>24</v>
       </c>
       <c r="D14" s="9">
-        <v>44068.000000000000</v>
+        <v>44069.000000000000</v>
       </c>
       <c r="E14" s="8">
         <v>153.90</v>
@@ -4317,7 +4315,7 @@
         <v>23</v>
       </c>
       <c r="D15" s="9">
-        <v>44069.000000000000</v>
+        <v>44070.000000000000</v>
       </c>
       <c r="E15" s="8">
         <v>8972.09</v>
@@ -4335,7 +4333,7 @@
         <v>25</v>
       </c>
       <c r="D16" s="9">
-        <v>44067.000000000000</v>
+        <v>44068.000000000000</v>
       </c>
       <c r="E16" s="8">
         <v>214.52</v>
@@ -4353,7 +4351,7 @@
         <v>24</v>
       </c>
       <c r="D17" s="9">
-        <v>44068.000000000000</v>
+        <v>44069.000000000000</v>
       </c>
       <c r="E17" s="8">
         <v>4164.85</v>
@@ -4371,7 +4369,7 @@
         <v>23</v>
       </c>
       <c r="D18" s="9">
-        <v>44069.000000000000</v>
+        <v>44070.000000000000</v>
       </c>
       <c r="E18" s="8">
         <v>847.44</v>
@@ -4389,7 +4387,7 @@
         <v>25</v>
       </c>
       <c r="D19" s="9">
-        <v>44067.000000000000</v>
+        <v>44068.000000000000</v>
       </c>
       <c r="E19" s="8">
         <v>6220.04</v>
@@ -4416,7 +4414,6 @@
     </row>
     <row r="21">
       <c r="A21" t="s"/>
-      <c r="A21"/>
       <c r="D21" s="20" t="s">
         <v>40</v>
       </c>
@@ -4485,7 +4482,7 @@
         <v>26</v>
       </c>
       <c r="D5" s="9">
-        <v>44066.000000000000</v>
+        <v>44067.000000000000</v>
       </c>
       <c r="E5" s="8">
         <v>6758.57</v>
@@ -4503,7 +4500,7 @@
         <v>26</v>
       </c>
       <c r="D6" s="9">
-        <v>44066.000000000000</v>
+        <v>44067.000000000000</v>
       </c>
       <c r="E6" s="8">
         <v>6836.72</v>
@@ -4521,7 +4518,7 @@
         <v>26</v>
       </c>
       <c r="D7" s="9">
-        <v>44066.000000000000</v>
+        <v>44067.000000000000</v>
       </c>
       <c r="E7" s="8">
         <v>4038.64</v>
@@ -4539,7 +4536,7 @@
         <v>26</v>
       </c>
       <c r="D8" s="9">
-        <v>44066.000000000000</v>
+        <v>44067.000000000000</v>
       </c>
       <c r="E8" s="8">
         <v>5746.69</v>
@@ -4557,7 +4554,7 @@
         <v>26</v>
       </c>
       <c r="D9" s="9">
-        <v>44066.000000000000</v>
+        <v>44067.000000000000</v>
       </c>
       <c r="E9" s="8">
         <v>471.62</v>
@@ -4589,7 +4586,7 @@
         <v>23</v>
       </c>
       <c r="D11" s="9">
-        <v>44069.000000000000</v>
+        <v>44070.000000000000</v>
       </c>
       <c r="E11" s="8">
         <v>982.68</v>
@@ -4607,7 +4604,7 @@
         <v>23</v>
       </c>
       <c r="D12" s="9">
-        <v>44069.000000000000</v>
+        <v>44070.000000000000</v>
       </c>
       <c r="E12" s="8">
         <v>7630.05</v>
@@ -4625,7 +4622,7 @@
         <v>23</v>
       </c>
       <c r="D13" s="9">
-        <v>44069.000000000000</v>
+        <v>44070.000000000000</v>
       </c>
       <c r="E13" s="8">
         <v>6001.36</v>
@@ -4643,7 +4640,7 @@
         <v>23</v>
       </c>
       <c r="D14" s="9">
-        <v>44069.000000000000</v>
+        <v>44070.000000000000</v>
       </c>
       <c r="E14" s="8">
         <v>8972.09</v>
@@ -4661,7 +4658,7 @@
         <v>23</v>
       </c>
       <c r="D15" s="9">
-        <v>44069.000000000000</v>
+        <v>44070.000000000000</v>
       </c>
       <c r="E15" s="8">
         <v>847.44</v>
@@ -4693,7 +4690,7 @@
         <v>25</v>
       </c>
       <c r="D17" s="9">
-        <v>44067.000000000000</v>
+        <v>44068.000000000000</v>
       </c>
       <c r="E17" s="8">
         <v>9950.90</v>
@@ -4711,7 +4708,7 @@
         <v>25</v>
       </c>
       <c r="D18" s="9">
-        <v>44067.000000000000</v>
+        <v>44068.000000000000</v>
       </c>
       <c r="E18" s="8">
         <v>214.52</v>
@@ -4729,7 +4726,7 @@
         <v>25</v>
       </c>
       <c r="D19" s="9">
-        <v>44067.000000000000</v>
+        <v>44068.000000000000</v>
       </c>
       <c r="E19" s="8">
         <v>6220.04</v>
@@ -4761,7 +4758,7 @@
         <v>24</v>
       </c>
       <c r="D21" s="9">
-        <v>44068.000000000000</v>
+        <v>44069.000000000000</v>
       </c>
       <c r="E21" s="8">
         <v>153.90</v>
@@ -4779,7 +4776,7 @@
         <v>24</v>
       </c>
       <c r="D22" s="9">
-        <v>44068.000000000000</v>
+        <v>44069.000000000000</v>
       </c>
       <c r="E22" s="8">
         <v>4164.85</v>
@@ -4872,7 +4869,7 @@
         <v>26</v>
       </c>
       <c r="C4" s="9">
-        <v>44066.000000000000</v>
+        <v>44067.000000000000</v>
       </c>
       <c r="D4" s="8">
         <v>6758.57</v>
@@ -4889,7 +4886,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="9">
-        <v>44069.000000000000</v>
+        <v>44070.000000000000</v>
       </c>
       <c r="D5" s="8">
         <v>982.68</v>
@@ -4906,7 +4903,7 @@
         <v>26</v>
       </c>
       <c r="C6" s="9">
-        <v>44066.000000000000</v>
+        <v>44067.000000000000</v>
       </c>
       <c r="D6" s="8">
         <v>6836.72</v>
@@ -4923,7 +4920,7 @@
         <v>26</v>
       </c>
       <c r="C7" s="9">
-        <v>44066.000000000000</v>
+        <v>44067.000000000000</v>
       </c>
       <c r="D7" s="8">
         <v>4038.64</v>
@@ -4940,7 +4937,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="9">
-        <v>44069.000000000000</v>
+        <v>44070.000000000000</v>
       </c>
       <c r="D8" s="8">
         <v>7630.05</v>
@@ -4957,7 +4954,7 @@
         <v>26</v>
       </c>
       <c r="C9" s="9">
-        <v>44066.000000000000</v>
+        <v>44067.000000000000</v>
       </c>
       <c r="D9" s="8">
         <v>5746.69</v>
@@ -4974,7 +4971,7 @@
         <v>26</v>
       </c>
       <c r="C10" s="9">
-        <v>44066.000000000000</v>
+        <v>44067.000000000000</v>
       </c>
       <c r="D10" s="8">
         <v>471.62</v>
@@ -4991,7 +4988,7 @@
         <v>23</v>
       </c>
       <c r="C11" s="9">
-        <v>44069.000000000000</v>
+        <v>44070.000000000000</v>
       </c>
       <c r="D11" s="8">
         <v>6001.36</v>
@@ -5008,7 +5005,7 @@
         <v>25</v>
       </c>
       <c r="C12" s="9">
-        <v>44067.000000000000</v>
+        <v>44068.000000000000</v>
       </c>
       <c r="D12" s="8">
         <v>9950.90</v>
@@ -5025,7 +5022,7 @@
         <v>24</v>
       </c>
       <c r="C13" s="9">
-        <v>44068.000000000000</v>
+        <v>44069.000000000000</v>
       </c>
       <c r="D13" s="8">
         <v>153.90</v>
@@ -5042,7 +5039,7 @@
         <v>23</v>
       </c>
       <c r="C14" s="9">
-        <v>44069.000000000000</v>
+        <v>44070.000000000000</v>
       </c>
       <c r="D14" s="8">
         <v>8972.09</v>
@@ -5059,7 +5056,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="9">
-        <v>44067.000000000000</v>
+        <v>44068.000000000000</v>
       </c>
       <c r="D15" s="8">
         <v>214.52</v>
@@ -5076,7 +5073,7 @@
         <v>24</v>
       </c>
       <c r="C16" s="9">
-        <v>44068.000000000000</v>
+        <v>44069.000000000000</v>
       </c>
       <c r="D16" s="8">
         <v>4164.85</v>
@@ -5093,7 +5090,7 @@
         <v>23</v>
       </c>
       <c r="C17" s="9">
-        <v>44069.000000000000</v>
+        <v>44070.000000000000</v>
       </c>
       <c r="D17" s="8">
         <v>847.44</v>
@@ -5110,7 +5107,7 @@
         <v>25</v>
       </c>
       <c r="C18" s="9">
-        <v>44067.000000000000</v>
+        <v>44068.000000000000</v>
       </c>
       <c r="D18" s="8">
         <v>6220.04</v>
@@ -5118,7 +5115,6 @@
       <c r="E18" s="8">
         <v>6482.36</v>
       </c>
-      <c r="E18"/>
     </row>
     <row r="22" customHeight="1" ht="15">
       <c r="E22" s="21" t="s">

</xml_diff>